<commit_message>
Preliminary commit for 0.2.0 release ====================================
* Renaming of Partition table to _Partition to cope with MISO-17, i.e. "Partition" is now a reserved keyword in MySQL 5.6 upwards.
* A lot of formatting changes to bring all Java and JS indentation etc together
* Inclusion of BarcodableSchemas to reduce the overhead for creating new print strategies
* Improvement in Project page loading times
* Improved Partition Container page - now includes pool list on the right, like the Run page
* Many miscellaneous bug fixes
</commit_message>
<xml_diff>
--- a/core/src/main/resources/forms/ods/bulk_input.xlsx
+++ b/core/src/main/resources/forms/ods/bulk_input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
   <si>
     <t>Paired</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Sample alias</t>
   </si>
   <si>
-    <t>Pool number</t>
-  </si>
-  <si>
-    <t>Sample QC</t>
-  </si>
-  <si>
     <t>Sample Vol</t>
   </si>
   <si>
@@ -58,9 +52,6 @@
     <t>Barcode tag</t>
   </si>
   <si>
-    <t>Library QC</t>
-  </si>
-  <si>
     <t>Insert size</t>
   </si>
   <si>
@@ -320,6 +311,42 @@
   </si>
   <si>
     <t>LS454-Rapid Shotgun</t>
+  </si>
+  <si>
+    <t>PacBio-10kb Shotgun</t>
+  </si>
+  <si>
+    <t>PacBio-20kb Shotgun</t>
+  </si>
+  <si>
+    <t>PacBio-2kb Shotgun</t>
+  </si>
+  <si>
+    <t>PacBio-Amplicon</t>
+  </si>
+  <si>
+    <t>PacBio-BAC</t>
+  </si>
+  <si>
+    <t>PacBio-Plasmid</t>
+  </si>
+  <si>
+    <t>PacBio-cDNA</t>
+  </si>
+  <si>
+    <t>Project Alias</t>
+  </si>
+  <si>
+    <t>Pool Alias</t>
+  </si>
+  <si>
+    <t>Sample QC Result</t>
+  </si>
+  <si>
+    <t>Library Description</t>
+  </si>
+  <si>
+    <t>Library QC type</t>
   </si>
 </sst>
 </file>
@@ -575,7 +602,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -596,9 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="7" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="7" fillId="8" borderId="3" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="7" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,6 +641,12 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="1" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="10" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="_1RC" xfId="1"/>
@@ -921,10 +952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMJ71"/>
+  <dimension ref="A1:AML71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -936,23 +967,24 @@
     <col min="5" max="5" width="26.375" style="4" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="4" customWidth="1"/>
     <col min="7" max="7" width="12.625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="13.125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="11.625" style="4" customWidth="1"/>
     <col min="11" max="11" width="21.5" style="4" customWidth="1"/>
     <col min="12" max="12" width="18" style="4" customWidth="1"/>
     <col min="13" max="13" width="19.875" style="4" customWidth="1"/>
     <col min="14" max="14" width="19.125" style="4" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="4" customWidth="1"/>
-    <col min="16" max="16" width="28" style="4" customWidth="1"/>
+    <col min="15" max="15" width="14.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.375" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="11.5" style="4" customWidth="1"/>
-    <col min="19" max="19" width="9.375" style="4" customWidth="1"/>
-    <col min="20" max="20" width="26.375" style="4" customWidth="1"/>
-    <col min="21" max="21" width="26.875" style="4" customWidth="1"/>
-    <col min="22" max="23" width="10" style="4" customWidth="1"/>
-    <col min="24" max="24" width="9.25" style="17" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.25" style="15" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="23.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.25" style="4" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="19.75" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="10" style="4" customWidth="1"/>
     <col min="29" max="29" width="13.375" style="4" customWidth="1"/>
@@ -960,7 +992,7 @@
     <col min="1024" max="1024" width="9" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:32 1025:1026">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,637 +1008,756 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="X1" s="4"/>
+      <c r="Y1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="Z1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC1" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="Y1" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30">
+      <c r="AMK1" s="4"/>
+      <c r="AML1" s="4"/>
+    </row>
+    <row r="2" spans="1:32 1025:1026">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
-      <c r="X2" s="5"/>
-      <c r="Y2"/>
-      <c r="Z2" s="17"/>
-      <c r="AA2" s="5"/>
-    </row>
-    <row r="3" spans="1:30">
-      <c r="W3" s="4" t="b">
+      <c r="X2" s="4"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="5"/>
+      <c r="AMK2" s="4"/>
+      <c r="AML2" s="4"/>
+    </row>
+    <row r="3" spans="1:32 1025:1026">
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="Z3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AA3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AMK3" s="4"/>
+      <c r="AML3" s="4"/>
+    </row>
+    <row r="4" spans="1:32 1025:1026">
+      <c r="A4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="W4" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AMK4" s="4"/>
+      <c r="AML4" s="4"/>
+    </row>
+    <row r="5" spans="1:32 1025:1026">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="I5" s="14"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="X5" s="4"/>
+      <c r="Z5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AMK5" s="4"/>
+      <c r="AML5" s="4"/>
+    </row>
+    <row r="6" spans="1:32 1025:1026">
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="I6" s="14"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="X6" s="4"/>
+      <c r="Z6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA6" t="s">
         <v>95</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="AB6" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="AA3" s="9" t="s">
+      <c r="AC6" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AC3"/>
-      <c r="AD3"/>
-    </row>
-    <row r="4" spans="1:30">
-      <c r="A4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="U4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="W4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="X4" s="9" t="s">
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AMK6" s="4"/>
+      <c r="AML6" s="4"/>
+    </row>
+    <row r="7" spans="1:32 1025:1026">
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="X7" s="4"/>
+      <c r="Z7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AA7" t="s">
         <v>96</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="AB7" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="9" t="s">
+      <c r="AC7" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="AC4"/>
-      <c r="AD4"/>
-    </row>
-    <row r="5" spans="1:30">
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="X5" s="9" t="s">
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AMK7" s="4"/>
+      <c r="AML7" s="4"/>
+    </row>
+    <row r="8" spans="1:32 1025:1026">
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="X8" s="4"/>
+      <c r="Z8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="Y5" t="s">
+      <c r="AA8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC8" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AMK8" s="4"/>
+      <c r="AML8" s="4"/>
+    </row>
+    <row r="9" spans="1:32 1025:1026">
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="X9" s="4"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AB9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AMK9" s="4"/>
+      <c r="AML9" s="4"/>
+    </row>
+    <row r="10" spans="1:32 1025:1026">
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="I10" s="14"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="X10" s="4"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AMK10" s="4"/>
+      <c r="AML10" s="4"/>
+    </row>
+    <row r="11" spans="1:32 1025:1026">
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="I11" s="14"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="X11" s="4"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AB11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AMK11" s="4"/>
+      <c r="AML11" s="4"/>
+    </row>
+    <row r="12" spans="1:32 1025:1026">
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="I12" s="14"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="X12" s="4"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AMK12" s="4"/>
+      <c r="AML12" s="4"/>
+    </row>
+    <row r="13" spans="1:32 1025:1026">
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="I13" s="14"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="X13" s="4"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" t="s">
         <v>97</v>
       </c>
-      <c r="Z5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC5"/>
-      <c r="AD5"/>
-    </row>
-    <row r="6" spans="1:30">
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="I6" s="16"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="X6" s="9" t="s">
+      <c r="AB13" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC13" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AMK13" s="4"/>
+      <c r="AML13" s="4"/>
+    </row>
+    <row r="14" spans="1:32 1025:1026">
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="I14" s="14"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="16"/>
+      <c r="S14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="X14" s="4"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC14" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AMK14" s="4"/>
+      <c r="AML14" s="4"/>
+    </row>
+    <row r="15" spans="1:32 1025:1026">
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="I15" s="14"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="X15" s="4"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AMK15" s="4"/>
+      <c r="AML15" s="4"/>
+    </row>
+    <row r="16" spans="1:32 1025:1026">
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="I16" s="14"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="X16" s="4"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB16" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AMK16" s="4"/>
+      <c r="AML16" s="4"/>
+    </row>
+    <row r="17" spans="5:32 1025:1026">
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="I17" s="14"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="X17" s="4"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB17" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC17" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AMK17" s="4"/>
+      <c r="AML17" s="4"/>
+    </row>
+    <row r="18" spans="5:32 1025:1026">
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="I18" s="14"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="X18" s="4"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC18" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AMK18" s="4"/>
+      <c r="AML18" s="4"/>
+    </row>
+    <row r="19" spans="5:32 1025:1026">
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="I19" s="14"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="X19" s="4"/>
+      <c r="Z19" s="15"/>
+      <c r="AA19" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC19" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AMK19" s="4"/>
+      <c r="AML19" s="4"/>
+    </row>
+    <row r="20" spans="5:32 1025:1026">
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="I20" s="14"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="X20" s="4"/>
+      <c r="Z20" s="15"/>
+      <c r="AA20" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC20" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="AMK20" s="4"/>
+      <c r="AML20" s="4"/>
+    </row>
+    <row r="21" spans="5:32 1025:1026">
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="I21" s="14"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="X21" s="4"/>
+      <c r="Z21" s="15"/>
+      <c r="AA21" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="AMK21" s="4"/>
+      <c r="AML21" s="4"/>
+    </row>
+    <row r="22" spans="5:32 1025:1026">
+      <c r="X22" s="4"/>
+      <c r="Z22" s="15"/>
+      <c r="AA22" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB22" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC22" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="AMK22" s="4"/>
+      <c r="AML22" s="4"/>
+    </row>
+    <row r="23" spans="5:32 1025:1026">
+      <c r="X23" s="4"/>
+      <c r="Z23" s="15"/>
+      <c r="AA23" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB23" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="AMK23" s="4"/>
+      <c r="AML23" s="4"/>
+    </row>
+    <row r="24" spans="5:32 1025:1026">
+      <c r="X24" s="4"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB24" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC24" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="AMK24" s="4"/>
+      <c r="AML24" s="4"/>
+    </row>
+    <row r="25" spans="5:32 1025:1026">
+      <c r="X25" s="4"/>
+      <c r="Z25" s="15"/>
+      <c r="AA25" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="Y6" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z6" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA6" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC6"/>
-      <c r="AD6"/>
-    </row>
-    <row r="7" spans="1:30">
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="I7" s="16"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
-      <c r="Q7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="X7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>99</v>
-      </c>
-      <c r="Z7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC7"/>
-      <c r="AD7"/>
-    </row>
-    <row r="8" spans="1:30">
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="I8" s="16"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="X8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z8" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA8" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AC8"/>
-      <c r="AD8"/>
-    </row>
-    <row r="9" spans="1:30">
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="I9" s="16"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="Y9" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z9" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA9" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC9"/>
-      <c r="AD9"/>
-    </row>
-    <row r="10" spans="1:30">
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="I10" s="16"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="X10" s="5"/>
-      <c r="Y10" t="s">
-        <v>92</v>
-      </c>
-      <c r="Z10" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA10" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC10"/>
-      <c r="AD10"/>
-    </row>
-    <row r="11" spans="1:30">
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="I11" s="16"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA11" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC11"/>
-      <c r="AD11"/>
-    </row>
-    <row r="12" spans="1:30">
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="I12" s="16"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" t="s">
-        <v>94</v>
-      </c>
-      <c r="Z12" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA12" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC12"/>
-      <c r="AD12"/>
-    </row>
-    <row r="13" spans="1:30">
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="I13" s="16"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="U13" s="15"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" t="s">
-        <v>100</v>
-      </c>
-      <c r="Z13" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA13" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC13"/>
-      <c r="AD13"/>
-    </row>
-    <row r="14" spans="1:30">
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="I14" s="16"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA14" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="AC14"/>
-      <c r="AD14"/>
-    </row>
-    <row r="15" spans="1:30">
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="I15" s="16"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="X15" s="9"/>
-      <c r="Y15" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z15" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA15" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC15"/>
-      <c r="AD15"/>
-    </row>
-    <row r="16" spans="1:30">
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="I16" s="16"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="X16" s="9"/>
-      <c r="Y16" t="s">
-        <v>86</v>
-      </c>
-      <c r="Z16" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA16" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC16"/>
-      <c r="AD16"/>
-    </row>
-    <row r="17" spans="5:30">
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="I17" s="16"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="X17" s="9"/>
-      <c r="Y17" t="s">
-        <v>87</v>
-      </c>
-      <c r="Z17" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA17" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC17"/>
-      <c r="AD17"/>
-    </row>
-    <row r="18" spans="5:30">
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="I18" s="16"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="X18" s="9"/>
-      <c r="Y18" t="s">
-        <v>88</v>
-      </c>
-      <c r="Z18" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA18" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC18"/>
-      <c r="AD18"/>
-    </row>
-    <row r="19" spans="5:30">
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="I19" s="16"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="Y19" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA19" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="AC19"/>
-      <c r="AD19"/>
-    </row>
-    <row r="20" spans="5:30">
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="I20" s="16"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="Y20"/>
-      <c r="Z20" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA20" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="5:30">
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="I21" s="16"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="Y21"/>
-      <c r="Z21" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA21" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="5:30">
-      <c r="Y22"/>
-      <c r="Z22" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA22" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="5:30">
-      <c r="Y23"/>
-      <c r="Z23" s="9" t="s">
+      <c r="AMK25" s="4"/>
+      <c r="AML25" s="4"/>
+    </row>
+    <row r="26" spans="5:32 1025:1026">
+      <c r="X26" s="4"/>
+      <c r="Z26" s="15"/>
+      <c r="AA26" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB26" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="AA23" s="9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="5:30">
-      <c r="Y24"/>
-      <c r="Z24" s="9" t="s">
+      <c r="AMK26" s="4"/>
+      <c r="AML26" s="4"/>
+    </row>
+    <row r="27" spans="5:32 1025:1026">
+      <c r="X27" s="4"/>
+      <c r="Z27" s="15"/>
+      <c r="AA27"/>
+      <c r="AB27" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="AA24" s="9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="5:30">
-      <c r="Y25"/>
-      <c r="Z25" s="9" t="s">
+      <c r="AMK27" s="4"/>
+      <c r="AML27" s="4"/>
+    </row>
+    <row r="28" spans="5:32 1025:1026">
+      <c r="X28" s="4"/>
+      <c r="Z28" s="15"/>
+      <c r="AA28"/>
+      <c r="AB28" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="AA25" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="5:30">
-      <c r="Y26"/>
-      <c r="Z26" s="9" t="s">
+      <c r="AMK28" s="4"/>
+      <c r="AML28" s="4"/>
+    </row>
+    <row r="29" spans="5:32 1025:1026">
+      <c r="X29" s="4"/>
+      <c r="Z29" s="15"/>
+      <c r="AA29"/>
+      <c r="AB29" s="9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="27" spans="5:30">
-      <c r="Y27"/>
-      <c r="Z27" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="5:30">
-      <c r="Y28"/>
-      <c r="Z28" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="5:30">
-      <c r="Y29"/>
-      <c r="Z29" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="30" spans="5:30">
+      <c r="AMK29" s="4"/>
+      <c r="AML29" s="4"/>
+    </row>
+    <row r="30" spans="5:32 1025:1026">
       <c r="Y30"/>
     </row>
-    <row r="31" spans="5:30">
+    <row r="31" spans="5:32 1025:1026">
       <c r="Y31"/>
     </row>
-    <row r="32" spans="5:30">
+    <row r="32" spans="5:32 1025:1026">
       <c r="Y32"/>
     </row>
     <row r="33" spans="25:25">
@@ -1725,20 +1876,20 @@
     </row>
   </sheetData>
   <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
+      <formula1>$Y$2:$Y$4</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>$X$2:$X$8</formula1>
+      <formula1>$Z$2:$Z$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
-      <formula1>$Y$2:$Y$19</formula1>
+      <formula1>$AA$2:$AA$26</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
-      <formula1>$Z$2:$Z$29</formula1>
+      <formula1>$AB$2:$AB$29</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
-      <formula1>$AA$2:$AA$25</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
-      <formula1>$W$3:$W$4</formula1>
+      <formula1>$AC$2:$AC$25</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>

</xml_diff>

<commit_message>
* help tab now directs to documentation confluence * changed spacing of body * plate export form now work on column based order * brand-new dashboard * new requestmanager api for getting samples by received date * Fix for NPE in MisoPrintService default and custom implementations. Also improved exception propagation when this happens
</commit_message>
<xml_diff>
--- a/core/src/main/resources/forms/ods/bulk_input.xlsx
+++ b/core/src/main/resources/forms/ods/bulk_input.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23812"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="495" windowWidth="19800" windowHeight="8115"/>
+    <workbookView xWindow="35000" yWindow="160" windowWidth="33600" windowHeight="19780"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <t>Paired</t>
   </si>
@@ -334,9 +339,6 @@
     <t>PacBio-cDNA</t>
   </si>
   <si>
-    <t>Project Alias</t>
-  </si>
-  <si>
     <t>Pool Alias</t>
   </si>
   <si>
@@ -347,19 +349,25 @@
   </si>
   <si>
     <t>Library QC type</t>
+  </si>
+  <si>
+    <t>Plate Barcode</t>
+  </si>
+  <si>
+    <t>Project Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="[$-809]General"/>
     <numFmt numFmtId="165" formatCode="[$-809]0.00"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
     <numFmt numFmtId="167" formatCode="[$£-809]#,##0.00;[Red]&quot;-&quot;[$£-809]#,##0.00"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -951,14 +959,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.625" style="4" customWidth="1"/>
     <col min="2" max="2" width="22.25" style="4" customWidth="1"/>
@@ -1008,6 +1016,9 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="X1" s="4"/>
       <c r="Y1" s="18" t="s">
         <v>0</v>
@@ -1068,16 +1079,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C4" s="21" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="22" t="s">
         <v>107</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>108</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>8</v>
@@ -1086,7 +1097,7 @@
         <v>9</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>10</v>
@@ -1095,7 +1106,7 @@
         <v>11</v>
       </c>
       <c r="K4" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L4" s="21" t="s">
         <v>12</v>
@@ -1893,7 +1904,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="1.1437007874015748" bottom="1.1437007874015748" header="0.75" footer="0.75"/>
-  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>